<commit_message>
Modify happy and angry
</commit_message>
<xml_diff>
--- a/dataset/angry.xlsx
+++ b/dataset/angry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이세미\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\semi\AdvancedML_project\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFEA490-1EED-4EA8-A397-79A28F8E47AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453F93DB-794B-48CB-B3EF-82723B09846B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12532" uniqueCount="6267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12506" uniqueCount="6254">
   <si>
     <t>우분투 그놈</t>
   </si>
@@ -385,9 +385,6 @@
     <t>남자친구 모욕죄나 명예회손죄로 신고</t>
   </si>
   <si>
-    <t xml:space="preserve">드라마 본대로 말하라 그놈 체포 시청자... </t>
-  </si>
-  <si>
     <t xml:space="preserve">이 사건...제가 명예훼손 죄나 모욕 죄로... </t>
   </si>
   <si>
@@ -1519,9 +1516,6 @@
     <t>새벽에 계속 짖어대는 미친개와 미친주인</t>
   </si>
   <si>
-    <t xml:space="preserve">드라마 발칙한여자에서 사강남편분... </t>
-  </si>
-  <si>
     <t>질투와시기</t>
   </si>
   <si>
@@ -1699,12 +1693,6 @@
     <t>부모는 자식이 개새끼여도 키우고 싶은</t>
   </si>
   <si>
-    <t xml:space="preserve">빌어먹을 세상 따위 같은 드라마/영화... </t>
-  </si>
-  <si>
-    <t>그놈이그놈이다 황정음신발 뭘까요</t>
-  </si>
-  <si>
     <t>딸아이가 유독 저한테만 신경질을 냅니다</t>
   </si>
   <si>
@@ -3889,9 +3877,6 @@
     <t xml:space="preserve">분한에 맞서는 군인 오빠언니들과 군인... </t>
   </si>
   <si>
-    <t>더폰 특종 그놈이다</t>
-  </si>
-  <si>
     <t>같은반에싸가지없는애때문에</t>
   </si>
   <si>
@@ -5020,9 +5005,6 @@
     <t>제가 그렇게 싸가지 없나요??</t>
   </si>
   <si>
-    <t xml:space="preserve">어벙하고,얄미운 며느리 나오는 드라마나... </t>
-  </si>
-  <si>
     <t xml:space="preserve">직장내 폭언 명예훼손 및 모욕죄... </t>
   </si>
   <si>
@@ -7582,9 +7564,6 @@
     <t>삐친친구와 화해하기</t>
   </si>
   <si>
-    <t>그놈이 그놈이다 황정음씨 가방 어디건가요</t>
-  </si>
-  <si>
     <t>이새끼 뭐죠? ㅋㅋㅋㅋㅋㅋㅋㅋ</t>
   </si>
   <si>
@@ -8893,9 +8872,6 @@
     <t>..... 짜증난...</t>
   </si>
   <si>
-    <t>왜 그놈이그놈이다는 되는데</t>
-  </si>
-  <si>
     <t xml:space="preserve">지랄머리(돼지털 곱슬)가 생머리로... </t>
   </si>
   <si>
@@ -11275,9 +11251,6 @@
     <t>싸가지 없는 친구가요...</t>
   </si>
   <si>
-    <t>그놈은 여고생 드라마화</t>
-  </si>
-  <si>
     <t>아빠갈기갈기찢어버릴거다</t>
   </si>
   <si>
@@ -13645,9 +13618,6 @@
     <t>SNS 명예훼손 및 모욕 관련 고소 방법</t>
   </si>
   <si>
-    <t>그놈이 그놈이다 황정음 가방 어디껀지?</t>
-  </si>
-  <si>
     <t>싸가지없는말투랑특이한말투좀요</t>
   </si>
   <si>
@@ -15415,9 +15385,6 @@
     <t>게임 내 모욕 사이버 명예훼손 각하</t>
   </si>
   <si>
-    <t>드라마 그놈이그놈이다 황정음지갑</t>
-  </si>
-  <si>
     <t xml:space="preserve">동생이 같은반 친구들에게 치욕적인 일을... </t>
   </si>
   <si>
@@ -16300,9 +16267,6 @@
     <t>타~타다다당다당탕당 이 치사한 자식</t>
   </si>
   <si>
-    <t>그놈이다랑 검은사제들 내공100</t>
-  </si>
-  <si>
     <t>무는 지랄견 ㅡㅡ</t>
   </si>
   <si>
@@ -17195,9 +17159,6 @@
   </si>
   <si>
     <t>싸가지 없는애 복수하는 방법</t>
-  </si>
-  <si>
-    <t>드라마나쁜남자 모네년!!!!!!!</t>
   </si>
   <si>
     <t>1년전 모욕사건 민사 가능한가요?</t>
@@ -19175,10 +19136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6266"/>
+  <dimension ref="A1:B6253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A5405" workbookViewId="0">
+      <selection activeCell="A5427" activeCellId="5" sqref="A557 A1286 A2519 A2957 A4542 A5427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -32876,7 +32837,7 @@
     </row>
     <row r="1712" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1712" t="s">
-        <v>1712</v>
+        <v>6253</v>
       </c>
       <c r="B1712" t="s">
         <v>1</v>
@@ -32884,7 +32845,7 @@
     </row>
     <row r="1713" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1713" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B1713" t="s">
         <v>1</v>
@@ -32892,7 +32853,7 @@
     </row>
     <row r="1714" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1714" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B1714" t="s">
         <v>1</v>
@@ -32900,7 +32861,7 @@
     </row>
     <row r="1715" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1715" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B1715" t="s">
         <v>1</v>
@@ -32908,7 +32869,7 @@
     </row>
     <row r="1716" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1716" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B1716" t="s">
         <v>1</v>
@@ -32916,7 +32877,7 @@
     </row>
     <row r="1717" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1717" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B1717" t="s">
         <v>1</v>
@@ -32924,7 +32885,7 @@
     </row>
     <row r="1718" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1718" t="s">
-        <v>6266</v>
+        <v>1717</v>
       </c>
       <c r="B1718" t="s">
         <v>1</v>
@@ -38588,7 +38549,7 @@
     </row>
     <row r="2426" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2426" t="s">
-        <v>2425</v>
+        <v>6252</v>
       </c>
       <c r="B2426" t="s">
         <v>1</v>
@@ -38596,7 +38557,7 @@
     </row>
     <row r="2427" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2427" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="B2427" t="s">
         <v>1</v>
@@ -38604,7 +38565,7 @@
     </row>
     <row r="2428" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2428" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="B2428" t="s">
         <v>1</v>
@@ -38612,7 +38573,7 @@
     </row>
     <row r="2429" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2429" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="B2429" t="s">
         <v>1</v>
@@ -38620,7 +38581,7 @@
     </row>
     <row r="2430" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2430" t="s">
-        <v>2429</v>
+        <v>6251</v>
       </c>
       <c r="B2430" t="s">
         <v>1</v>
@@ -38628,7 +38589,7 @@
     </row>
     <row r="2431" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2431" t="s">
-        <v>2430</v>
+        <v>2428</v>
       </c>
       <c r="B2431" t="s">
         <v>1</v>
@@ -38636,7 +38597,7 @@
     </row>
     <row r="2432" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2432" t="s">
-        <v>6265</v>
+        <v>2429</v>
       </c>
       <c r="B2432" t="s">
         <v>1</v>
@@ -38644,7 +38605,7 @@
     </row>
     <row r="2433" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2433" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="B2433" t="s">
         <v>1</v>
@@ -38652,7 +38613,7 @@
     </row>
     <row r="2434" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2434" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="B2434" t="s">
         <v>1</v>
@@ -38660,7 +38621,7 @@
     </row>
     <row r="2435" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2435" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="B2435" t="s">
         <v>1</v>
@@ -38668,7 +38629,7 @@
     </row>
     <row r="2436" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2436" t="s">
-        <v>6264</v>
+        <v>2433</v>
       </c>
       <c r="B2436" t="s">
         <v>1</v>
@@ -42260,7 +42221,7 @@
     </row>
     <row r="2885" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2885" t="s">
-        <v>2882</v>
+        <v>6250</v>
       </c>
       <c r="B2885" t="s">
         <v>1</v>
@@ -42268,7 +42229,7 @@
     </row>
     <row r="2886" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2886" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="B2886" t="s">
         <v>1</v>
@@ -42276,7 +42237,7 @@
     </row>
     <row r="2887" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2887" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
       <c r="B2887" t="s">
         <v>1</v>
@@ -42284,7 +42245,7 @@
     </row>
     <row r="2888" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2888" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
       <c r="B2888" t="s">
         <v>1</v>
@@ -42292,7 +42253,7 @@
     </row>
     <row r="2889" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2889" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
       <c r="B2889" t="s">
         <v>1</v>
@@ -42300,7 +42261,7 @@
     </row>
     <row r="2890" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2890" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
       <c r="B2890" t="s">
         <v>1</v>
@@ -42308,7 +42269,7 @@
     </row>
     <row r="2891" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2891" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="B2891" t="s">
         <v>1</v>
@@ -42316,7 +42277,7 @@
     </row>
     <row r="2892" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2892" t="s">
-        <v>6263</v>
+        <v>2888</v>
       </c>
       <c r="B2892" t="s">
         <v>1</v>
@@ -49596,7 +49557,7 @@
     </row>
     <row r="3802" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3802" t="s">
-        <v>3798</v>
+        <v>6249</v>
       </c>
       <c r="B3802" t="s">
         <v>1</v>
@@ -49604,7 +49565,7 @@
     </row>
     <row r="3803" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3803" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="B3803" t="s">
         <v>1</v>
@@ -49612,7 +49573,7 @@
     </row>
     <row r="3804" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3804" t="s">
-        <v>3800</v>
+        <v>3799</v>
       </c>
       <c r="B3804" t="s">
         <v>1</v>
@@ -49620,7 +49581,7 @@
     </row>
     <row r="3805" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3805" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="B3805" t="s">
         <v>1</v>
@@ -49628,7 +49589,7 @@
     </row>
     <row r="3806" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3806" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="B3806" t="s">
         <v>1</v>
@@ -49636,7 +49597,7 @@
     </row>
     <row r="3807" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3807" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="B3807" t="s">
         <v>1</v>
@@ -49644,7 +49605,7 @@
     </row>
     <row r="3808" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3808" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="B3808" t="s">
         <v>1</v>
@@ -49652,7 +49613,7 @@
     </row>
     <row r="3809" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3809" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="B3809" t="s">
         <v>1</v>
@@ -49660,7 +49621,7 @@
     </row>
     <row r="3810" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3810" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="B3810" t="s">
         <v>1</v>
@@ -49668,7 +49629,7 @@
     </row>
     <row r="3811" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3811" t="s">
-        <v>6262</v>
+        <v>3806</v>
       </c>
       <c r="B3811" t="s">
         <v>1</v>
@@ -53588,7 +53549,7 @@
     </row>
     <row r="4301" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4301" t="s">
-        <v>4296</v>
+        <v>6248</v>
       </c>
       <c r="B4301" t="s">
         <v>1</v>
@@ -53596,7 +53557,7 @@
     </row>
     <row r="4302" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4302" t="s">
-        <v>4297</v>
+        <v>4296</v>
       </c>
       <c r="B4302" t="s">
         <v>1</v>
@@ -53604,7 +53565,7 @@
     </row>
     <row r="4303" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4303" t="s">
-        <v>4298</v>
+        <v>4297</v>
       </c>
       <c r="B4303" t="s">
         <v>1</v>
@@ -53612,7 +53573,7 @@
     </row>
     <row r="4304" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4304" t="s">
-        <v>4299</v>
+        <v>4298</v>
       </c>
       <c r="B4304" t="s">
         <v>1</v>
@@ -53620,7 +53581,7 @@
     </row>
     <row r="4305" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4305" t="s">
-        <v>4300</v>
+        <v>4299</v>
       </c>
       <c r="B4305" t="s">
         <v>1</v>
@@ -53628,7 +53589,7 @@
     </row>
     <row r="4306" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4306" t="s">
-        <v>4301</v>
+        <v>4300</v>
       </c>
       <c r="B4306" t="s">
         <v>1</v>
@@ -53636,7 +53597,7 @@
     </row>
     <row r="4307" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4307" t="s">
-        <v>4302</v>
+        <v>4301</v>
       </c>
       <c r="B4307" t="s">
         <v>1</v>
@@ -53644,7 +53605,7 @@
     </row>
     <row r="4308" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4308" t="s">
-        <v>4303</v>
+        <v>4302</v>
       </c>
       <c r="B4308" t="s">
         <v>1</v>
@@ -53652,7 +53613,7 @@
     </row>
     <row r="4309" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4309" t="s">
-        <v>4304</v>
+        <v>4303</v>
       </c>
       <c r="B4309" t="s">
         <v>1</v>
@@ -53660,7 +53621,7 @@
     </row>
     <row r="4310" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4310" t="s">
-        <v>6261</v>
+        <v>4304</v>
       </c>
       <c r="B4310" t="s">
         <v>1</v>
@@ -61924,7 +61885,7 @@
     </row>
     <row r="5343" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5343" t="s">
-        <v>5337</v>
+        <v>6247</v>
       </c>
       <c r="B5343" t="s">
         <v>1</v>
@@ -61932,7 +61893,7 @@
     </row>
     <row r="5344" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5344" t="s">
-        <v>5338</v>
+        <v>5337</v>
       </c>
       <c r="B5344" t="s">
         <v>1</v>
@@ -61940,7 +61901,7 @@
     </row>
     <row r="5345" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5345" t="s">
-        <v>5339</v>
+        <v>5338</v>
       </c>
       <c r="B5345" t="s">
         <v>1</v>
@@ -61948,7 +61909,7 @@
     </row>
     <row r="5346" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5346" t="s">
-        <v>5340</v>
+        <v>5339</v>
       </c>
       <c r="B5346" t="s">
         <v>1</v>
@@ -61956,7 +61917,7 @@
     </row>
     <row r="5347" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5347" t="s">
-        <v>5341</v>
+        <v>5340</v>
       </c>
       <c r="B5347" t="s">
         <v>1</v>
@@ -61964,7 +61925,7 @@
     </row>
     <row r="5348" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5348" t="s">
-        <v>5342</v>
+        <v>5341</v>
       </c>
       <c r="B5348" t="s">
         <v>1</v>
@@ -61972,7 +61933,7 @@
     </row>
     <row r="5349" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5349" t="s">
-        <v>5343</v>
+        <v>5342</v>
       </c>
       <c r="B5349" t="s">
         <v>1</v>
@@ -61980,7 +61941,7 @@
     </row>
     <row r="5350" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5350" t="s">
-        <v>5344</v>
+        <v>5343</v>
       </c>
       <c r="B5350" t="s">
         <v>1</v>
@@ -61988,7 +61949,7 @@
     </row>
     <row r="5351" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5351" t="s">
-        <v>5345</v>
+        <v>5344</v>
       </c>
       <c r="B5351" t="s">
         <v>1</v>
@@ -61996,7 +61957,7 @@
     </row>
     <row r="5352" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5352" t="s">
-        <v>5346</v>
+        <v>5345</v>
       </c>
       <c r="B5352" t="s">
         <v>1</v>
@@ -62004,7 +61965,7 @@
     </row>
     <row r="5353" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5353" t="s">
-        <v>5347</v>
+        <v>5346</v>
       </c>
       <c r="B5353" t="s">
         <v>1</v>
@@ -62012,7 +61973,7 @@
     </row>
     <row r="5354" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5354" t="s">
-        <v>6260</v>
+        <v>5347</v>
       </c>
       <c r="B5354" t="s">
         <v>1</v>
@@ -69207,110 +69168,6 @@
         <v>6246</v>
       </c>
       <c r="B6253" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6254" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6254" t="s">
-        <v>6247</v>
-      </c>
-      <c r="B6254" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6255" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6255" t="s">
-        <v>6248</v>
-      </c>
-      <c r="B6255" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6256" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6256" t="s">
-        <v>6249</v>
-      </c>
-      <c r="B6256" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6257" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6257" t="s">
-        <v>6250</v>
-      </c>
-      <c r="B6257" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6258" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6258" t="s">
-        <v>6251</v>
-      </c>
-      <c r="B6258" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6259" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6259" t="s">
-        <v>6252</v>
-      </c>
-      <c r="B6259" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6260" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6260" t="s">
-        <v>6253</v>
-      </c>
-      <c r="B6260" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6261" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6261" t="s">
-        <v>6254</v>
-      </c>
-      <c r="B6261" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6262" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6262" t="s">
-        <v>6255</v>
-      </c>
-      <c r="B6262" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6263" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6263" t="s">
-        <v>6256</v>
-      </c>
-      <c r="B6263" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6264" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6264" t="s">
-        <v>6257</v>
-      </c>
-      <c r="B6264" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6265" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6265" t="s">
-        <v>6258</v>
-      </c>
-      <c r="B6265" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6266" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6266" t="s">
-        <v>6259</v>
-      </c>
-      <c r="B6266" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>